<commit_message>
[Karthik] Modified collect tax feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="chequeDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -142,6 +142,7 @@
       <color rgb="FF008000"/>
       <name val="DejaVu Sans Mono"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,17 +223,17 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -281,18 +282,18 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.5407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="16.437037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="16.9407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="16.7555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -371,11 +372,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.737037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.9296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.8851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[Vinay] Completed the Scenario Register Choose to do title Transfer
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="chequeDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -109,9 +109,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -187,16 +188,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -223,17 +228,17 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="H:H C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -282,21 +287,22 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H:H"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.52592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="16.7555555555556"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.1481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>6</v>
       </c>
@@ -318,15 +324,15 @@
       <c r="G1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>42710</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -344,7 +350,7 @@
       <c r="G2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>500</v>
       </c>
     </row>
@@ -367,26 +373,26 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="1" sqref="H:H E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.8851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.862962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="0" t="s">

</xml_diff>

<commit_message>
[PHOENIX-5881] Modified some changes
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="chequeDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -102,7 +102,7 @@
     <t xml:space="preserve">Senior Assistant</t>
   </si>
   <si>
-    <t xml:space="preserve">P.Mahaboob Basha-ADM_Senior Assistant_5</t>
+    <t xml:space="preserve">K.Ramakrishna-ADM_Senior Assistant_7</t>
   </si>
 </sst>
 </file>
@@ -234,9 +234,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -285,19 +287,19 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -370,17 +372,17 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.9222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-5880] Modified Miscellaneous receipt scenario
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="chequeDetails" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="challanHeaderDetails" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="approvalDetails" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="paymentMethod" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -103,6 +104,27 @@
   </si>
   <si>
     <t xml:space="preserve">K.Ramakrishna-ADM_Senior Assistant_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dd/chequeNum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cheque</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">credit/debit card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">direct bank</t>
   </si>
 </sst>
 </file>
@@ -234,11 +256,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -287,19 +309,19 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="19.5"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -372,17 +394,17 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2814814814815"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.3296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -411,6 +433,90 @@
       </c>
       <c r="D2" s="0" t="s">
         <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62222222222222"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PHOENIX-5880] Modified Miscellanous receipt
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -109,6 +109,9 @@
     <t xml:space="preserve">dd/chequeNum</t>
   </si>
   <si>
+    <t xml:space="preserve">accountNum</t>
+  </si>
+  <si>
     <t xml:space="preserve">cash</t>
   </si>
   <si>
@@ -124,7 +127,13 @@
     <t xml:space="preserve">credit/debit card</t>
   </si>
   <si>
-    <t xml:space="preserve">direct bank</t>
+    <t xml:space="preserve">directBank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATE BANK OF HYDERABAD-KMC Complex Kurnool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62007226282</t>
   </si>
 </sst>
 </file>
@@ -256,11 +265,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -315,13 +324,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.8"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.8"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.4814814814815"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -400,11 +409,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.3296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -451,21 +460,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.7407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>6</v>
       </c>
@@ -475,21 +485,27 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>123456</v>
@@ -497,10 +513,13 @@
       <c r="C3" s="0" t="n">
         <v>102</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>123456</v>
@@ -508,15 +527,27 @@
       <c r="C4" s="0" t="n">
         <v>102</v>
       </c>
+      <c r="D4" s="0" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PHOENIX-5879] Added bill based receipt and rearranged all scenarios
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t xml:space="preserve">62007226282</t>
+  </si>
+  <si>
+    <t xml:space="preserve">directBank1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATE BANK OF INDIA-SBI Tresury Branch, Kurnool</t>
   </si>
 </sst>
 </file>
@@ -219,7 +225,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -238,6 +244,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -265,11 +275,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -324,13 +334,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.4814814814815"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.9703703703704"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -409,11 +419,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.6814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.5333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.9555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,19 +470,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -548,6 +558,20 @@
       </c>
       <c r="D6" s="1" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>123987</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>844810206002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PHOENIX-5999] Modified for qa environment
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
@@ -130,10 +130,10 @@
     <t xml:space="preserve">directBank</t>
   </si>
   <si>
-    <t xml:space="preserve">STATE BANK OF HYDERABAD-KMC Complex Kurnool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62007226282</t>
+    <t xml:space="preserve">ANDHRA BANK-Andhra Bank RTC Busstand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110710011005899</t>
   </si>
   <si>
     <t xml:space="preserve">directBank1</t>
@@ -275,11 +275,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.8"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,13 +334,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -419,11 +419,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.337037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.5333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.9555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.3185185185185"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.2296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -473,16 +473,16 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-5858] Done some changes for qa environment
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
@@ -275,11 +275,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,13 +334,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.5851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -419,11 +419,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.1222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.3185185185185"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.2296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.9074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.1037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.5037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -473,16 +473,16 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-5999] refactoring the entire module
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/CollectionsTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="chequeDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -275,11 +275,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,13 +334,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="22.0481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="22.537037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,17 +413,17 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.9074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.1037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.5037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.6888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.9851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.8777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,17 +472,17 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>